<commit_message>
500 exp with 15,20 agents
</commit_message>
<xml_diff>
--- a/results_submaps/cu_bso/30x30/cu_bso_30x30_True_2_500.xlsx
+++ b/results_submaps/cu_bso/30x30/cu_bso_30x30_True_2_500.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1156,6 +1156,218 @@
         <v>0.85</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>15</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>29.09</v>
+      </c>
+      <c r="D14" t="n">
+        <v>435.548</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.97736638</v>
+      </c>
+      <c r="F14" t="n">
+        <v>20564362.12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.29189352</v>
+      </c>
+      <c r="H14" t="n">
+        <v>15.78603854</v>
+      </c>
+      <c r="I14" t="n">
+        <v>461.9314859</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.549648183892288</v>
+      </c>
+      <c r="K14" t="n">
+        <v>68.09076589965487</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.3042690013133379</v>
+      </c>
+      <c r="M14" t="n">
+        <v>7747045.444773559</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1.576608731235504</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2.399488369536128</v>
+      </c>
+      <c r="P14" t="n">
+        <v>116.2805947480786</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>43.16</v>
+      </c>
+      <c r="D15" t="n">
+        <v>632.6799999999999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.3564264</v>
+      </c>
+      <c r="F15" t="n">
+        <v>25707741.752</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11.63860912</v>
+      </c>
+      <c r="H15" t="n">
+        <v>32.91796542</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1428.68794184</v>
+      </c>
+      <c r="J15" t="n">
+        <v>6.669885662400743</v>
+      </c>
+      <c r="K15" t="n">
+        <v>93.46923877508787</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.1885996524334975</v>
+      </c>
+      <c r="M15" t="n">
+        <v>8483622.617616583</v>
+      </c>
+      <c r="N15" t="n">
+        <v>3.003980909877465</v>
+      </c>
+      <c r="O15" t="n">
+        <v>7.576114327711927</v>
+      </c>
+      <c r="P15" t="n">
+        <v>433.9464282085918</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>20</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>21.694</v>
+      </c>
+      <c r="D16" t="n">
+        <v>432.682</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.99801192</v>
+      </c>
+      <c r="F16" t="n">
+        <v>34295968.112</v>
+      </c>
+      <c r="G16" t="n">
+        <v>10.0291708</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10.69102954</v>
+      </c>
+      <c r="I16" t="n">
+        <v>234.3309088</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3.624726373474987</v>
+      </c>
+      <c r="K16" t="n">
+        <v>72.16139834303132</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.3335295188101783</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10749485.79427716</v>
+      </c>
+      <c r="N16" t="n">
+        <v>3.201314198864626</v>
+      </c>
+      <c r="O16" t="n">
+        <v>3.272110775208575</v>
+      </c>
+      <c r="P16" t="n">
+        <v>89.66405358001231</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>20</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>33.416</v>
+      </c>
+      <c r="D17" t="n">
+        <v>645.302</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.33802164</v>
+      </c>
+      <c r="F17" t="n">
+        <v>48130139.712</v>
+      </c>
+      <c r="G17" t="n">
+        <v>11.79523276</v>
+      </c>
+      <c r="H17" t="n">
+        <v>19.30532634</v>
+      </c>
+      <c r="I17" t="n">
+        <v>650.48072802</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5.830517461403874</v>
+      </c>
+      <c r="K17" t="n">
+        <v>106.7509171512135</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.2153220606796737</v>
+      </c>
+      <c r="M17" t="n">
+        <v>15414344.87170735</v>
+      </c>
+      <c r="N17" t="n">
+        <v>3.448034262654486</v>
+      </c>
+      <c r="O17" t="n">
+        <v>5.232150290690965</v>
+      </c>
+      <c r="P17" t="n">
+        <v>229.6351214302819</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>